<commit_message>
Fixed JSON and MeOH model.
</commit_message>
<xml_diff>
--- a/Matt_Work/Methanol Growth/2015_06_05_manual met adding.xlsx
+++ b/Matt_Work/Methanol Growth/2015_06_05_manual met adding.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="22995" windowHeight="11055"/>
+    <workbookView xWindow="240" yWindow="132" windowWidth="15576" windowHeight="9816"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Reaction</t>
   </si>
@@ -115,6 +115,12 @@
   </si>
   <si>
     <t>100 v 1</t>
+  </si>
+  <si>
+    <t>100 v 1 w/ antiport</t>
+  </si>
+  <si>
+    <t>rxn05209_c0</t>
   </si>
 </sst>
 </file>
@@ -492,32 +498,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W13"/>
+  <dimension ref="A1:W15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="2"/>
-    <col min="5" max="6" width="9.140625" style="4"/>
-    <col min="8" max="8" width="9.140625" style="4"/>
-    <col min="11" max="13" width="9.140625" style="3"/>
-    <col min="16" max="16" width="9.140625" style="5"/>
-    <col min="17" max="17" width="9.140625" style="3"/>
-    <col min="19" max="20" width="9.140625" style="6"/>
-    <col min="22" max="22" width="9.140625" style="2"/>
+    <col min="3" max="4" width="9.109375" style="2"/>
+    <col min="5" max="6" width="9.109375" style="4"/>
+    <col min="8" max="8" width="9.109375" style="4"/>
+    <col min="11" max="13" width="9.109375" style="3"/>
+    <col min="16" max="16" width="9.109375" style="5"/>
+    <col min="17" max="17" width="9.109375" style="3"/>
+    <col min="19" max="20" width="9.109375" style="6"/>
+    <col min="22" max="22" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -588,7 +594,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -659,7 +665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -730,7 +736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -801,7 +807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -872,7 +878,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -943,7 +949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -1014,7 +1020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -1085,7 +1091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -1156,95 +1162,235 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0</v>
+      </c>
+      <c r="F12" s="4">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12" s="4">
+        <v>0</v>
+      </c>
+      <c r="I12" s="4">
+        <v>0</v>
+      </c>
+      <c r="J12" s="4">
+        <v>0</v>
+      </c>
+      <c r="K12" s="3">
+        <v>0</v>
+      </c>
+      <c r="L12" s="3">
+        <v>0</v>
+      </c>
+      <c r="M12" s="3">
+        <v>0</v>
+      </c>
+      <c r="N12" s="3">
+        <v>0</v>
+      </c>
+      <c r="O12" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>32</v>
       </c>
-      <c r="B13">
+      <c r="B14">
         <f>100*B4 + 99*B5 + 99*B6 + 98*B7 + 48.5*B8+SUM(B9:B11)</f>
         <v>0</v>
       </c>
-      <c r="C13">
-        <f t="shared" ref="C13:W13" si="0">100*C4 + 99*C5 + 99*C6 + 98*C7 + 48.5*C8+SUM(C9:C11)</f>
+      <c r="C14">
+        <f>100*C4 + 99*C5 + 99*C6 + 98*C7 + 48.5*C8+SUM(C9:C11)</f>
         <v>-48.5</v>
       </c>
-      <c r="D13">
-        <f t="shared" si="0"/>
+      <c r="D14">
+        <f>100*D4 + 99*D5 + 99*D6 + 98*D7 + 48.5*D8+SUM(D9:D11)</f>
         <v>48.5</v>
       </c>
-      <c r="E13">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-      <c r="G13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-      <c r="I13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K13">
-        <f t="shared" si="0"/>
+      <c r="E14">
+        <f>100*E4 + 99*E5 + 99*E6 + 98*E7 + 48.5*E8+SUM(E9:E11)</f>
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <f>100*F4 + 99*F5 + 99*F6 + 98*F7 + 48.5*F8+SUM(F9:F11)</f>
+        <v>-1</v>
+      </c>
+      <c r="G14">
+        <f>100*G4 + 99*G5 + 99*G6 + 98*G7 + 48.5*G8+SUM(G9:G11)</f>
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <f>100*H4 + 99*H5 + 99*H6 + 98*H7 + 48.5*H8+SUM(H9:H11)</f>
+        <v>-1</v>
+      </c>
+      <c r="I14">
+        <f>100*I4 + 99*I5 + 99*I6 + 98*I7 + 48.5*I8+SUM(I9:I11)</f>
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <f>100*J4 + 99*J5 + 99*J6 + 98*J7 + 48.5*J8+SUM(J9:J11)</f>
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <f>100*K4 + 99*K5 + 99*K6 + 98*K7 + 48.5*K8+SUM(K9:K11)</f>
         <v>99</v>
       </c>
-      <c r="L13">
-        <f t="shared" si="0"/>
+      <c r="L14">
+        <f>100*L4 + 99*L5 + 99*L6 + 98*L7 + 48.5*L8+SUM(L9:L11)</f>
         <v>148.5</v>
       </c>
-      <c r="M13">
-        <f t="shared" si="0"/>
+      <c r="M14">
+        <f>100*M4 + 99*M5 + 99*M6 + 98*M7 + 48.5*M8+SUM(M9:M11)</f>
         <v>-100</v>
       </c>
-      <c r="N13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P13" s="5">
-        <f t="shared" si="0"/>
+      <c r="N14">
+        <f>100*N4 + 99*N5 + 99*N6 + 98*N7 + 48.5*N8+SUM(N9:N11)</f>
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <f>100*O4 + 99*O5 + 99*O6 + 98*O7 + 48.5*O8+SUM(O9:O11)</f>
+        <v>0</v>
+      </c>
+      <c r="P14" s="5">
+        <f>100*P4 + 99*P5 + 99*P6 + 98*P7 + 48.5*P8+SUM(P9:P11)</f>
         <v>-148.5</v>
       </c>
-      <c r="Q13">
-        <f t="shared" si="0"/>
+      <c r="Q14">
+        <f>100*Q4 + 99*Q5 + 99*Q6 + 98*Q7 + 48.5*Q8+SUM(Q9:Q11)</f>
         <v>-100</v>
       </c>
-      <c r="R13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="S13" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="T13" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="U13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="V13">
-        <f t="shared" si="0"/>
+      <c r="R14">
+        <f>100*R4 + 99*R5 + 99*R6 + 98*R7 + 48.5*R8+SUM(R9:R11)</f>
+        <v>0</v>
+      </c>
+      <c r="S14" s="6">
+        <f>100*S4 + 99*S5 + 99*S6 + 98*S7 + 48.5*S8+SUM(S9:S11)</f>
+        <v>0</v>
+      </c>
+      <c r="T14" s="6">
+        <f>100*T4 + 99*T5 + 99*T6 + 98*T7 + 48.5*T8+SUM(T9:T11)</f>
+        <v>0</v>
+      </c>
+      <c r="U14">
+        <f>100*U4 + 99*U5 + 99*U6 + 98*U7 + 48.5*U8+SUM(U9:U11)</f>
+        <v>0</v>
+      </c>
+      <c r="V14">
+        <f>100*V4 + 99*V5 + 99*V6 + 98*V7 + 48.5*V8+SUM(V9:V11)</f>
         <v>-48.5</v>
       </c>
-      <c r="W13">
+      <c r="W14">
+        <f>100*W4 + 99*W5 + 99*W6 + 98*W7 + 48.5*W8+SUM(W9:W11)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15">
+        <f>100*B4 + 99*B5 + 99*B6 + 98*B7 + 48.5*B8+SUM(B9:B11)</f>
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <f t="shared" ref="C15:W15" si="0">100*C4 + 99*C5 + 99*C6 + 98*C7 + 48.5*C8+SUM(C9:C11)</f>
+        <v>-48.5</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>48.5</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="0"/>
+        <v>99</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>148.5</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="0"/>
+        <v>-148.5</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V15">
+        <f t="shared" si="0"/>
+        <v>-48.5</v>
+      </c>
+      <c r="W15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1261,7 +1407,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1273,7 +1419,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>